<commit_message>
Arbeit Freitag 10.12 ISFH
Asuwertung python ...
</commit_message>
<xml_diff>
--- a/Masterarbeit/Auswertungen/Datensammlung_diemangebrauchenkann.xlsx
+++ b/Masterarbeit/Auswertungen/Datensammlung_diemangebrauchenkann.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bomml\Documents\GitHub\Master-s-Thesis\Masterarbeit\Auswertungen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.oberroehrmann\Documents\GitHub\Master-s-Thesis\Masterarbeit\Auswertungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E422B5-6F63-4119-BF3A-A9C09412C6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B8B9A2-08AE-41C2-A35A-A1DC294ACE0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15510" yWindow="1725" windowWidth="11280" windowHeight="11385" activeTab="1" xr2:uid="{944C2AFD-4F65-408D-8CFA-E731EA682F22}"/>
   </bookViews>
@@ -22,21 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="152">
   <si>
     <t>Parameters and Units</t>
   </si>
@@ -477,6 +468,21 @@
   </si>
   <si>
     <t>DOS (cm^-3)</t>
+  </si>
+  <si>
+    <t>Zelllänge [cm]</t>
+  </si>
+  <si>
+    <t>Flächenwiderstand ITO [Ohm]</t>
+  </si>
+  <si>
+    <t>Freies ITO bis Metallisierung [cm]</t>
+  </si>
+  <si>
+    <t>Serienwiderstand durch ITO [Ohmcm²]</t>
+  </si>
+  <si>
+    <t>Spezifischer Widerstand ITO [Ohm*m]</t>
   </si>
 </sst>
 </file>
@@ -498,7 +504,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,6 +523,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -807,7 +819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -834,9 +846,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -854,6 +863,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1304,53 +1319,53 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29">
+      <c r="B3" s="27"/>
+      <c r="C3" s="28">
         <v>-4.3</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="28">
         <v>-2.23</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="28">
         <v>-3.9</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="28">
         <v>-3.5</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="28">
         <v>-5.9</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="28">
         <v>-5.3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33">
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32">
         <f>D5-D3</f>
         <v>-2.9200000000000004</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="32">
         <f t="shared" ref="E4:G4" si="0">E5-E3</f>
         <v>-1.5000000000000004</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="32">
         <f t="shared" si="0"/>
         <v>-3.5</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="32">
         <f t="shared" si="0"/>
         <v>1.7000000000000002</v>
       </c>
-      <c r="H4" s="33"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
@@ -1576,13 +1591,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36608D0C-FFD4-4A19-B24D-E7D3B3061D26}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,79 +1607,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="35" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42"/>
-      <c r="B2" s="35" t="s">
+    <row r="2" spans="1:7" s="34" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41"/>
+      <c r="B2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="34" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="37">
         <v>100</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="37">
         <v>100</v>
       </c>
-      <c r="D3" s="38">
+      <c r="D3" s="37">
         <v>10</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="38">
         <v>500</v>
       </c>
-      <c r="F3" s="39">
+      <c r="F3" s="38">
         <v>8</v>
       </c>
-      <c r="G3" s="39">
+      <c r="G3" s="38">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="37">
         <f>B3*0.0000001</f>
         <v>9.9999999999999991E-6</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="37">
         <f t="shared" ref="C4:G4" si="0">C3*0.0000001</f>
         <v>9.9999999999999991E-6</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="37">
         <f t="shared" si="0"/>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="37">
         <f t="shared" si="0"/>
         <v>4.9999999999999996E-5</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="37">
         <f t="shared" si="0"/>
         <v>7.9999999999999996E-7</v>
       </c>
-      <c r="G4" s="38">
+      <c r="G4" s="37">
         <f t="shared" si="0"/>
         <v>2.3E-6</v>
       </c>
@@ -1676,10 +1691,10 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="36">
         <v>0.05</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="36">
         <v>1.5999999999999999E-5</v>
       </c>
     </row>
@@ -1687,22 +1702,22 @@
       <c r="A6" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E6" s="37">
+      <c r="E6" s="36">
         <v>1E-13</v>
       </c>
-      <c r="F6" s="37"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="36">
         <v>1.97E-3</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="36">
         <v>0.05</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="36">
         <v>1.6000000000000001E-4</v>
       </c>
       <c r="G7">
@@ -1713,16 +1728,16 @@
       <c r="A8" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="36">
         <v>1E-4</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="36">
         <v>1.6000000000000001E-4</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="36">
         <v>2.0000000000000001E-9</v>
       </c>
     </row>
@@ -1801,12 +1816,12 @@
       <c r="A13" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="39">
         <v>-3.93</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G14" s="40">
+      <c r="G14" s="39">
         <v>-4.32</v>
       </c>
     </row>
@@ -1819,7 +1834,7 @@
       <c r="A16" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E16" s="37">
+      <c r="E16" s="36">
         <v>8.1E+24</v>
       </c>
     </row>
@@ -1832,7 +1847,7 @@
       <c r="A18" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="E18" s="37">
+      <c r="E18" s="36">
         <v>8.1E+24</v>
       </c>
     </row>
@@ -1840,7 +1855,7 @@
       <c r="A19" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="E19" s="37">
+      <c r="E19" s="36">
         <f>E18*0.000001</f>
         <v>8.1E+18</v>
       </c>
@@ -1871,18 +1886,18 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="36"/>
+      <c r="D22" s="35"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D23" s="43">
+      <c r="D23" s="42">
         <v>1.8E-5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="43">
+      <c r="D24" s="42">
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
@@ -1921,6 +1936,51 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+      <c r="B33" s="45"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>151</v>
+      </c>
+      <c r="B34" s="46">
+        <v>1.5120000000000001E-6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" s="44">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>149</v>
+      </c>
+      <c r="B37" s="44">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38">
+        <f>(1/3*B36+B37)*B36*B35</f>
+        <v>4.4800000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -2026,7 +2086,7 @@
       <c r="C11" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="43" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2037,7 +2097,7 @@
       <c r="C12" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="26"/>
+      <c r="D12" s="43"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2086,7 +2146,7 @@
       <c r="B18" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="43" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2097,7 +2157,7 @@
       <c r="B19" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="26"/>
+      <c r="D19" s="43"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">

</xml_diff>